<commit_message>
# Actualize seccion de Metricas y Cronograma en el Project Plan
</commit_message>
<xml_diff>
--- a/meetings/Costos.20100927.xlsx
+++ b/meetings/Costos.20100927.xlsx
@@ -330,7 +330,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>22.5</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -340,11 +340,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="92270592"/>
-        <c:axId val="92272512"/>
+        <c:axId val="104333312"/>
+        <c:axId val="104335232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92270592"/>
+        <c:axId val="104333312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -370,14 +370,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92272512"/>
+        <c:crossAx val="104335232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92272512"/>
+        <c:axId val="104335232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,7 +404,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92270592"/>
+        <c:crossAx val="104333312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -417,7 +417,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -761,7 +761,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -805,7 +805,7 @@
         <v>72</v>
       </c>
       <c r="D3" s="3">
-        <v>22.5</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4">

</xml_diff>